<commit_message>
Updating the notification files
</commit_message>
<xml_diff>
--- a/data/excelsheets/statenotificationscalculations.xlsx
+++ b/data/excelsheets/statenotificationscalculations.xlsx
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="21">
   <si>
     <t>NN</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>Updated data (using national rate for HCV notifications where there aren't any)</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -906,11 +909,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="909509632"/>
-        <c:axId val="221077504"/>
+        <c:axId val="176063616"/>
+        <c:axId val="176065152"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="909509632"/>
+        <c:axId val="176063616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -952,7 +955,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="221077504"/>
+        <c:crossAx val="176065152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -960,7 +963,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="221077504"/>
+        <c:axId val="176065152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1011,7 +1014,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="909509632"/>
+        <c:crossAx val="176063616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1975,10 +1978,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z48"/>
+  <dimension ref="A1:Z70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B2"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51:J70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3751,7 +3754,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="42" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>2007</v>
       </c>
@@ -4246,6 +4249,819 @@
       </c>
       <c r="Z48" s="2">
         <v>412</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B51" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F51" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G51" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H51" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I51" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J51" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
+        <v>1995</v>
+      </c>
+      <c r="B52" s="2">
+        <f>B5+R30</f>
+        <v>336</v>
+      </c>
+      <c r="C52" s="2">
+        <f t="shared" ref="C52:J67" si="21">C5+S30</f>
+        <v>6590</v>
+      </c>
+      <c r="D52" s="2">
+        <f>D5</f>
+        <v>301</v>
+      </c>
+      <c r="E52" s="2">
+        <f>E5</f>
+        <v>2772</v>
+      </c>
+      <c r="F52" s="2">
+        <f t="shared" si="21"/>
+        <v>2226</v>
+      </c>
+      <c r="G52" s="2">
+        <f t="shared" si="21"/>
+        <v>253</v>
+      </c>
+      <c r="H52" s="2">
+        <f t="shared" si="21"/>
+        <v>1989</v>
+      </c>
+      <c r="I52" s="2">
+        <f>I5</f>
+        <v>1105</v>
+      </c>
+      <c r="J52" s="2">
+        <f t="shared" si="21"/>
+        <v>15572</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
+        <v>1996</v>
+      </c>
+      <c r="B53" s="2">
+        <f t="shared" ref="B53:B70" si="22">B6+R31</f>
+        <v>277</v>
+      </c>
+      <c r="C53" s="2">
+        <f t="shared" si="21"/>
+        <v>7087</v>
+      </c>
+      <c r="D53" s="2">
+        <f t="shared" ref="D53:E63" si="23">D6</f>
+        <v>214</v>
+      </c>
+      <c r="E53" s="2">
+        <f t="shared" si="23"/>
+        <v>2759</v>
+      </c>
+      <c r="F53" s="2">
+        <f t="shared" si="21"/>
+        <v>2451</v>
+      </c>
+      <c r="G53" s="2">
+        <f t="shared" si="21"/>
+        <v>259</v>
+      </c>
+      <c r="H53" s="2">
+        <f t="shared" si="21"/>
+        <v>2161</v>
+      </c>
+      <c r="I53" s="2">
+        <f t="shared" ref="I53:I61" si="24">I6</f>
+        <v>1049</v>
+      </c>
+      <c r="J53" s="2">
+        <f t="shared" si="21"/>
+        <v>16257</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
+        <v>1997</v>
+      </c>
+      <c r="B54" s="2">
+        <f t="shared" si="22"/>
+        <v>317</v>
+      </c>
+      <c r="C54" s="2">
+        <f t="shared" si="21"/>
+        <v>6486</v>
+      </c>
+      <c r="D54" s="2">
+        <f t="shared" si="23"/>
+        <v>295</v>
+      </c>
+      <c r="E54" s="2">
+        <f t="shared" si="23"/>
+        <v>2819</v>
+      </c>
+      <c r="F54" s="2">
+        <f t="shared" si="21"/>
+        <v>1905</v>
+      </c>
+      <c r="G54" s="2">
+        <f t="shared" si="21"/>
+        <v>201</v>
+      </c>
+      <c r="H54" s="2">
+        <f t="shared" si="21"/>
+        <v>2146</v>
+      </c>
+      <c r="I54" s="2">
+        <f t="shared" si="24"/>
+        <v>999</v>
+      </c>
+      <c r="J54" s="2">
+        <f t="shared" si="21"/>
+        <v>15168</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
+        <v>1998</v>
+      </c>
+      <c r="B55" s="2">
+        <f t="shared" si="22"/>
+        <v>298</v>
+      </c>
+      <c r="C55" s="2">
+        <f t="shared" si="21"/>
+        <v>6855</v>
+      </c>
+      <c r="D55" s="2">
+        <f t="shared" si="23"/>
+        <v>233</v>
+      </c>
+      <c r="E55" s="2">
+        <f t="shared" si="23"/>
+        <v>2876</v>
+      </c>
+      <c r="F55" s="2">
+        <f t="shared" si="21"/>
+        <v>1836</v>
+      </c>
+      <c r="G55" s="2">
+        <f t="shared" si="21"/>
+        <v>274</v>
+      </c>
+      <c r="H55" s="2">
+        <f t="shared" si="21"/>
+        <v>4184</v>
+      </c>
+      <c r="I55" s="2">
+        <f t="shared" si="24"/>
+        <v>1096</v>
+      </c>
+      <c r="J55" s="2">
+        <f t="shared" si="21"/>
+        <v>17652</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
+        <v>1999</v>
+      </c>
+      <c r="B56" s="2">
+        <f t="shared" si="22"/>
+        <v>301</v>
+      </c>
+      <c r="C56" s="2">
+        <f t="shared" si="21"/>
+        <v>7797</v>
+      </c>
+      <c r="D56" s="2">
+        <f t="shared" si="23"/>
+        <v>192</v>
+      </c>
+      <c r="E56" s="2">
+        <f t="shared" si="23"/>
+        <v>3004</v>
+      </c>
+      <c r="F56" s="2">
+        <f t="shared" si="21"/>
+        <v>1017</v>
+      </c>
+      <c r="G56" s="2">
+        <f t="shared" si="21"/>
+        <v>296</v>
+      </c>
+      <c r="H56" s="2">
+        <f t="shared" si="21"/>
+        <v>5617</v>
+      </c>
+      <c r="I56" s="2">
+        <f t="shared" si="24"/>
+        <v>980</v>
+      </c>
+      <c r="J56" s="2">
+        <f t="shared" si="21"/>
+        <v>19204</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
+        <v>2000</v>
+      </c>
+      <c r="B57" s="2">
+        <f t="shared" si="22"/>
+        <v>231</v>
+      </c>
+      <c r="C57" s="2">
+        <f t="shared" si="21"/>
+        <v>7357</v>
+      </c>
+      <c r="D57" s="2">
+        <f t="shared" si="23"/>
+        <v>189</v>
+      </c>
+      <c r="E57" s="2">
+        <f t="shared" si="23"/>
+        <v>3312</v>
+      </c>
+      <c r="F57" s="2">
+        <f t="shared" si="21"/>
+        <v>963</v>
+      </c>
+      <c r="G57" s="2">
+        <f t="shared" si="21"/>
+        <v>330</v>
+      </c>
+      <c r="H57" s="2">
+        <f t="shared" si="21"/>
+        <v>5113</v>
+      </c>
+      <c r="I57" s="2">
+        <f t="shared" si="24"/>
+        <v>1541</v>
+      </c>
+      <c r="J57" s="2">
+        <f t="shared" si="21"/>
+        <v>19036</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A58" s="1">
+        <v>2001</v>
+      </c>
+      <c r="B58" s="2">
+        <f t="shared" si="22"/>
+        <v>230</v>
+      </c>
+      <c r="C58" s="2">
+        <f t="shared" si="21"/>
+        <v>7769</v>
+      </c>
+      <c r="D58" s="2">
+        <f t="shared" si="23"/>
+        <v>214</v>
+      </c>
+      <c r="E58" s="2">
+        <f t="shared" si="23"/>
+        <v>2955</v>
+      </c>
+      <c r="F58" s="2">
+        <f t="shared" si="21"/>
+        <v>879</v>
+      </c>
+      <c r="G58" s="2">
+        <f t="shared" si="21"/>
+        <v>329</v>
+      </c>
+      <c r="H58" s="2">
+        <f t="shared" si="21"/>
+        <v>4603</v>
+      </c>
+      <c r="I58" s="2">
+        <f t="shared" si="24"/>
+        <v>1190</v>
+      </c>
+      <c r="J58" s="2">
+        <f t="shared" si="21"/>
+        <v>18169</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A59" s="1">
+        <v>2002</v>
+      </c>
+      <c r="B59" s="2">
+        <f t="shared" si="22"/>
+        <v>233</v>
+      </c>
+      <c r="C59" s="2">
+        <f t="shared" si="21"/>
+        <v>6165</v>
+      </c>
+      <c r="D59" s="2">
+        <f t="shared" si="23"/>
+        <v>200</v>
+      </c>
+      <c r="E59" s="2">
+        <f t="shared" si="23"/>
+        <v>2866</v>
+      </c>
+      <c r="F59" s="2">
+        <f t="shared" si="21"/>
+        <v>688</v>
+      </c>
+      <c r="G59" s="2">
+        <f t="shared" si="21"/>
+        <v>340</v>
+      </c>
+      <c r="H59" s="2">
+        <f t="shared" si="21"/>
+        <v>3783</v>
+      </c>
+      <c r="I59" s="2">
+        <f t="shared" si="24"/>
+        <v>989</v>
+      </c>
+      <c r="J59" s="2">
+        <f t="shared" si="21"/>
+        <v>15264</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A60" s="1">
+        <v>2003</v>
+      </c>
+      <c r="B60" s="2">
+        <f t="shared" si="22"/>
+        <v>253</v>
+      </c>
+      <c r="C60" s="2">
+        <f t="shared" si="21"/>
+        <v>4892</v>
+      </c>
+      <c r="D60" s="2">
+        <f t="shared" si="23"/>
+        <v>219</v>
+      </c>
+      <c r="E60" s="2">
+        <f t="shared" si="23"/>
+        <v>2590</v>
+      </c>
+      <c r="F60" s="2">
+        <f t="shared" si="21"/>
+        <v>660</v>
+      </c>
+      <c r="G60" s="2">
+        <f t="shared" si="21"/>
+        <v>353</v>
+      </c>
+      <c r="H60" s="2">
+        <f t="shared" si="21"/>
+        <v>3547</v>
+      </c>
+      <c r="I60" s="2">
+        <f t="shared" si="24"/>
+        <v>1064</v>
+      </c>
+      <c r="J60" s="2">
+        <f t="shared" si="21"/>
+        <v>13578</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A61" s="1">
+        <v>2004</v>
+      </c>
+      <c r="B61" s="2">
+        <f t="shared" si="22"/>
+        <v>216</v>
+      </c>
+      <c r="C61" s="2">
+        <f t="shared" si="21"/>
+        <v>4532</v>
+      </c>
+      <c r="D61" s="2">
+        <f t="shared" si="23"/>
+        <v>258</v>
+      </c>
+      <c r="E61" s="2">
+        <f t="shared" si="23"/>
+        <v>2633</v>
+      </c>
+      <c r="F61" s="2">
+        <f t="shared" si="21"/>
+        <v>673</v>
+      </c>
+      <c r="G61" s="2">
+        <f t="shared" si="21"/>
+        <v>309</v>
+      </c>
+      <c r="H61" s="2">
+        <f t="shared" si="21"/>
+        <v>3029</v>
+      </c>
+      <c r="I61" s="2">
+        <f t="shared" si="24"/>
+        <v>1030</v>
+      </c>
+      <c r="J61" s="2">
+        <f t="shared" si="21"/>
+        <v>12680</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A62" s="1">
+        <v>2005</v>
+      </c>
+      <c r="B62" s="2">
+        <f t="shared" si="22"/>
+        <v>173</v>
+      </c>
+      <c r="C62" s="2">
+        <f t="shared" si="21"/>
+        <v>4158</v>
+      </c>
+      <c r="D62" s="2">
+        <f t="shared" si="23"/>
+        <v>255</v>
+      </c>
+      <c r="E62" s="2">
+        <f t="shared" si="23"/>
+        <v>2623</v>
+      </c>
+      <c r="F62" s="2">
+        <f t="shared" si="21"/>
+        <v>603</v>
+      </c>
+      <c r="G62" s="2">
+        <f t="shared" si="21"/>
+        <v>240</v>
+      </c>
+      <c r="H62" s="2">
+        <f t="shared" si="21"/>
+        <v>2961</v>
+      </c>
+      <c r="I62" s="2">
+        <f t="shared" si="21"/>
+        <v>1055</v>
+      </c>
+      <c r="J62" s="2">
+        <f t="shared" si="21"/>
+        <v>12068</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A63" s="1">
+        <v>2006</v>
+      </c>
+      <c r="B63" s="2">
+        <f t="shared" si="22"/>
+        <v>192</v>
+      </c>
+      <c r="C63" s="2">
+        <f t="shared" si="21"/>
+        <v>4092</v>
+      </c>
+      <c r="D63" s="2">
+        <f t="shared" si="23"/>
+        <v>259</v>
+      </c>
+      <c r="E63" s="2">
+        <f t="shared" si="23"/>
+        <v>2821</v>
+      </c>
+      <c r="F63" s="2">
+        <f t="shared" si="21"/>
+        <v>570</v>
+      </c>
+      <c r="G63" s="2">
+        <f t="shared" si="21"/>
+        <v>271</v>
+      </c>
+      <c r="H63" s="2">
+        <f t="shared" si="21"/>
+        <v>2746</v>
+      </c>
+      <c r="I63" s="2">
+        <f t="shared" si="21"/>
+        <v>1106</v>
+      </c>
+      <c r="J63" s="2">
+        <f t="shared" si="21"/>
+        <v>12057</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A64" s="1">
+        <v>2007</v>
+      </c>
+      <c r="B64" s="2">
+        <f t="shared" si="22"/>
+        <v>199</v>
+      </c>
+      <c r="C64" s="2">
+        <f t="shared" si="21"/>
+        <v>4131</v>
+      </c>
+      <c r="D64" s="2">
+        <f t="shared" si="21"/>
+        <v>229</v>
+      </c>
+      <c r="E64" s="2">
+        <f t="shared" ref="E64" si="25">E17</f>
+        <v>2647</v>
+      </c>
+      <c r="F64" s="2">
+        <f t="shared" si="21"/>
+        <v>627</v>
+      </c>
+      <c r="G64" s="2">
+        <f t="shared" si="21"/>
+        <v>273</v>
+      </c>
+      <c r="H64" s="2">
+        <f t="shared" si="21"/>
+        <v>2759</v>
+      </c>
+      <c r="I64" s="2">
+        <f t="shared" si="21"/>
+        <v>1235</v>
+      </c>
+      <c r="J64" s="2">
+        <f t="shared" si="21"/>
+        <v>12100</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A65" s="1">
+        <v>2008</v>
+      </c>
+      <c r="B65" s="2">
+        <f t="shared" si="22"/>
+        <v>201</v>
+      </c>
+      <c r="C65" s="2">
+        <f t="shared" si="21"/>
+        <v>3425</v>
+      </c>
+      <c r="D65" s="2">
+        <f t="shared" si="21"/>
+        <v>209</v>
+      </c>
+      <c r="E65" s="2">
+        <f t="shared" ref="E65" si="26">E18</f>
+        <v>2602</v>
+      </c>
+      <c r="F65" s="2">
+        <f t="shared" si="21"/>
+        <v>611</v>
+      </c>
+      <c r="G65" s="2">
+        <f t="shared" si="21"/>
+        <v>349</v>
+      </c>
+      <c r="H65" s="2">
+        <f t="shared" si="21"/>
+        <v>2413</v>
+      </c>
+      <c r="I65" s="2">
+        <f t="shared" si="21"/>
+        <v>1355</v>
+      </c>
+      <c r="J65" s="2">
+        <f t="shared" si="21"/>
+        <v>11165</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A66" s="1">
+        <v>2009</v>
+      </c>
+      <c r="B66" s="2">
+        <f t="shared" si="22"/>
+        <v>163</v>
+      </c>
+      <c r="C66" s="2">
+        <f t="shared" si="21"/>
+        <v>4053</v>
+      </c>
+      <c r="D66" s="2">
+        <f t="shared" si="21"/>
+        <v>168</v>
+      </c>
+      <c r="E66" s="2">
+        <f t="shared" ref="E66" si="27">E19</f>
+        <v>2632</v>
+      </c>
+      <c r="F66" s="2">
+        <f t="shared" si="21"/>
+        <v>563</v>
+      </c>
+      <c r="G66" s="2">
+        <f t="shared" si="21"/>
+        <v>281</v>
+      </c>
+      <c r="H66" s="2">
+        <f t="shared" si="21"/>
+        <v>2500</v>
+      </c>
+      <c r="I66" s="2">
+        <f t="shared" si="21"/>
+        <v>1138</v>
+      </c>
+      <c r="J66" s="2">
+        <f t="shared" si="21"/>
+        <v>11498</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A67" s="1">
+        <v>2010</v>
+      </c>
+      <c r="B67" s="2">
+        <f t="shared" si="22"/>
+        <v>223</v>
+      </c>
+      <c r="C67" s="2">
+        <f t="shared" si="21"/>
+        <v>3979</v>
+      </c>
+      <c r="D67" s="2">
+        <f t="shared" si="21"/>
+        <v>169</v>
+      </c>
+      <c r="E67" s="2">
+        <f t="shared" ref="E67" si="28">E20</f>
+        <v>2671</v>
+      </c>
+      <c r="F67" s="2">
+        <f t="shared" si="21"/>
+        <v>534</v>
+      </c>
+      <c r="G67" s="2">
+        <f t="shared" si="21"/>
+        <v>267</v>
+      </c>
+      <c r="H67" s="2">
+        <f t="shared" si="21"/>
+        <v>2575</v>
+      </c>
+      <c r="I67" s="2">
+        <f t="shared" si="21"/>
+        <v>1065</v>
+      </c>
+      <c r="J67" s="2">
+        <f t="shared" si="21"/>
+        <v>11483</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A68" s="1">
+        <v>2011</v>
+      </c>
+      <c r="B68" s="2">
+        <f t="shared" si="22"/>
+        <v>189</v>
+      </c>
+      <c r="C68" s="2">
+        <f t="shared" ref="C68:C70" si="29">C21+S46</f>
+        <v>3372</v>
+      </c>
+      <c r="D68" s="2">
+        <f t="shared" ref="D68:D70" si="30">D21+T46</f>
+        <v>208</v>
+      </c>
+      <c r="E68" s="2">
+        <f t="shared" ref="E68" si="31">E21</f>
+        <v>2407</v>
+      </c>
+      <c r="F68" s="2">
+        <f t="shared" ref="F68:F70" si="32">F21+V46</f>
+        <v>474</v>
+      </c>
+      <c r="G68" s="2">
+        <f t="shared" ref="G68:G70" si="33">G21+W46</f>
+        <v>229</v>
+      </c>
+      <c r="H68" s="2">
+        <f t="shared" ref="H68:H70" si="34">H21+X46</f>
+        <v>2329</v>
+      </c>
+      <c r="I68" s="2">
+        <f t="shared" ref="I68:I70" si="35">I21+Y46</f>
+        <v>1083</v>
+      </c>
+      <c r="J68" s="2">
+        <f t="shared" ref="J68:J70" si="36">J21+Z46</f>
+        <v>10291</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A69" s="1">
+        <v>2012</v>
+      </c>
+      <c r="B69" s="2">
+        <f t="shared" si="22"/>
+        <v>147</v>
+      </c>
+      <c r="C69" s="2">
+        <f t="shared" si="29"/>
+        <v>3277</v>
+      </c>
+      <c r="D69" s="2">
+        <f t="shared" si="30"/>
+        <v>191</v>
+      </c>
+      <c r="E69" s="2">
+        <f t="shared" ref="E69" si="37">E22</f>
+        <v>2384</v>
+      </c>
+      <c r="F69" s="2">
+        <f t="shared" si="32"/>
+        <v>487</v>
+      </c>
+      <c r="G69" s="2">
+        <f t="shared" si="33"/>
+        <v>262</v>
+      </c>
+      <c r="H69" s="2">
+        <f t="shared" si="34"/>
+        <v>2240</v>
+      </c>
+      <c r="I69" s="2">
+        <f t="shared" si="35"/>
+        <v>1139</v>
+      </c>
+      <c r="J69" s="2">
+        <f t="shared" si="36"/>
+        <v>10127</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A70" s="1">
+        <v>2013</v>
+      </c>
+      <c r="B70" s="2">
+        <f t="shared" si="22"/>
+        <v>184</v>
+      </c>
+      <c r="C70" s="2">
+        <f t="shared" si="29"/>
+        <v>3550</v>
+      </c>
+      <c r="D70" s="2">
+        <f t="shared" si="30"/>
+        <v>257</v>
+      </c>
+      <c r="E70" s="2">
+        <f t="shared" ref="E70" si="38">E23</f>
+        <v>2467</v>
+      </c>
+      <c r="F70" s="2">
+        <f t="shared" si="32"/>
+        <v>476</v>
+      </c>
+      <c r="G70" s="2">
+        <f t="shared" si="33"/>
+        <v>229</v>
+      </c>
+      <c r="H70" s="2">
+        <f t="shared" si="34"/>
+        <v>2277</v>
+      </c>
+      <c r="I70" s="2">
+        <f t="shared" si="35"/>
+        <v>1278</v>
+      </c>
+      <c r="J70" s="2">
+        <f t="shared" si="36"/>
+        <v>10718</v>
       </c>
     </row>
   </sheetData>

</xml_diff>